<commit_message>
Commited In VSCODE 28/06
</commit_message>
<xml_diff>
--- a/Banco-de-Dados/Aula14-06/Exercicio-Excel.xlsx
+++ b/Banco-de-Dados/Aula14-06/Exercicio-Excel.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GUSTAVORIBEIRODASILV\Documents\SENAC\Back End\aula-senac\Banco-de-Dados\Aula14-06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B35DD9-B96C-4BA7-810B-3D53F2FDCE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C4B39E-DE1B-40DE-BE02-1112EFE6AD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{BAABA69F-8CA9-4481-80C9-C1F1C0723D84}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
-    <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
-    <sheet name="Planilha5" sheetId="5" r:id="rId5"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Pedidos" sheetId="2" r:id="rId2"/>
+    <sheet name="Produtos" sheetId="3" r:id="rId3"/>
+    <sheet name="Itens Pedido" sheetId="4" r:id="rId4"/>
+    <sheet name="Pagamento" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,9 +58,6 @@
     <t>Valor Total</t>
   </si>
   <si>
-    <t>ID do Pedido</t>
-  </si>
-  <si>
     <t>ID do Produto</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Id do Produto (Chave Estrangeira)</t>
+  </si>
+  <si>
+    <t>ID do Pedido (Chave Estrangeira)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +218,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -232,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -243,6 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -561,7 +568,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,10 +597,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>51977227277</v>
@@ -604,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>51903324567</v>
@@ -618,10 +625,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>51945535670</v>
@@ -632,10 +639,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>51935123561</v>
@@ -646,10 +653,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>51925626840</v>
@@ -685,16 +692,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -780,7 +787,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,16 +801,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -811,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -822,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -839,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -850,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>100</v>
@@ -861,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -877,7 +884,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,22 +898,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1004,14 +1011,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.54296875" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="16.36328125" customWidth="1"/>
@@ -1019,22 +1026,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1045,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1062,7 +1069,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -1079,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -1096,7 +1103,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -1113,7 +1120,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>30</v>

</xml_diff>